<commit_message>
pumped storage and bio-mass
</commit_message>
<xml_diff>
--- a/virginia/data/scenarios_multiple.xlsx
+++ b/virginia/data/scenarios_multiple.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6FE24F-824D-2D4D-BE99-EE9339D2324F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCCB13F-2D84-6A48-8D86-703E58A5BEFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8640" yWindow="2660" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="65">
   <si>
     <t>Scenario</t>
   </si>
@@ -212,6 +212,12 @@
   </si>
   <si>
     <t>NUCLEAR</t>
+  </si>
+  <si>
+    <t>EX_PUMP</t>
+  </si>
+  <si>
+    <t>EC_PUMP</t>
   </si>
 </sst>
 </file>
@@ -534,7 +540,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -666,7 +672,7 @@
         <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -677,10 +683,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -833,7 +839,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
@@ -844,7 +850,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
         <v>27</v>
@@ -855,23 +861,29 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
         <v>27</v>
@@ -879,7 +891,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
         <v>27</v>
@@ -887,7 +899,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
         <v>27</v>
@@ -895,29 +907,23 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
         <v>27</v>
@@ -928,7 +934,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
@@ -939,39 +945,61 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>